<commit_message>
solved 1st part of scenario 2
</commit_message>
<xml_diff>
--- a/Assignment 1/EGI_2024_A1_numerics.xlsx
+++ b/Assignment 1/EGI_2024_A1_numerics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mauriciorodriguez/Dropbox/TiU-MR/Lecturer/1_BSc-TiU_EGI/Assignments/2024/A1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakub\Documents\studies\subjects\4-semester\macro 4\Assignments\Assignment 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6885DB3F-EADD-F24B-B98E-3EBB6166614A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ECE719D-AE53-48CB-9B48-FDFCBA2D8D6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4380" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="6" r:id="rId1"/>
@@ -848,7 +848,7 @@
     </font>
     <font>
       <b/>
-      <sz val="14"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -1234,51 +1234,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AV120"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" style="1"/>
-    <col min="2" max="2" width="9.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.1640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" style="1"/>
+    <col min="2" max="2" width="9.1796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.1796875" style="1" customWidth="1"/>
     <col min="4" max="4" width="8" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" style="1" customWidth="1"/>
-    <col min="8" max="10" width="9.1640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="17.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.36328125" style="1" customWidth="1"/>
+    <col min="8" max="10" width="9.1796875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="17.1796875" style="1" customWidth="1"/>
     <col min="12" max="12" width="8" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.5" style="1" customWidth="1"/>
-    <col min="14" max="14" width="13.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.83203125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="9.1640625" style="1"/>
-    <col min="18" max="18" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="13.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18.33203125" style="1" customWidth="1"/>
-    <col min="23" max="23" width="9.1640625" style="1"/>
-    <col min="24" max="24" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.5" style="1" customWidth="1"/>
-    <col min="26" max="26" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.453125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="13.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.81640625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="9.1796875" style="1"/>
+    <col min="18" max="18" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="13.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.36328125" style="1" customWidth="1"/>
+    <col min="23" max="23" width="9.1796875" style="1"/>
+    <col min="24" max="24" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.453125" style="1" customWidth="1"/>
+    <col min="26" max="26" width="9.6328125" style="1" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="9" style="1" customWidth="1"/>
-    <col min="28" max="28" width="9.1640625" style="1"/>
-    <col min="29" max="29" width="10.5" style="1" customWidth="1"/>
-    <col min="30" max="30" width="13.1640625" style="1" customWidth="1"/>
-    <col min="31" max="31" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9.1640625" style="1" customWidth="1"/>
-    <col min="33" max="33" width="18.83203125" style="1" customWidth="1"/>
-    <col min="34" max="34" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.1796875" style="1"/>
+    <col min="29" max="29" width="10.453125" style="1" customWidth="1"/>
+    <col min="30" max="30" width="13.1796875" style="1" customWidth="1"/>
+    <col min="31" max="31" width="11.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9.1796875" style="1" customWidth="1"/>
+    <col min="33" max="33" width="18.81640625" style="1" customWidth="1"/>
+    <col min="34" max="34" width="9.6328125" style="1" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="13" style="1" bestFit="1" customWidth="1"/>
     <col min="36" max="37" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="9.1640625" style="1"/>
-    <col min="40" max="40" width="10.1640625" style="1" customWidth="1"/>
-    <col min="41" max="41" width="11.6640625" style="1" customWidth="1"/>
-    <col min="42" max="16384" width="9.1640625" style="1"/>
+    <col min="39" max="39" width="9.1796875" style="1"/>
+    <col min="40" max="40" width="10.1796875" style="1" customWidth="1"/>
+    <col min="41" max="41" width="11.6328125" style="1" customWidth="1"/>
+    <col min="42" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C1" s="14"/>
       <c r="E1" s="16" t="s">
         <v>47</v>
@@ -1357,7 +1359,7 @@
       <c r="AJ1" s="16"/>
       <c r="AP1" s="2"/>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.3">
       <c r="C2" s="15"/>
       <c r="F2" s="1">
         <v>0.25</v>
@@ -1424,21 +1426,21 @@
       <c r="AS2" s="5"/>
       <c r="AT2" s="4"/>
     </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.3">
       <c r="C3" s="14"/>
       <c r="K3" s="14"/>
       <c r="V3" s="14"/>
       <c r="AG3" s="14"/>
       <c r="AS3" s="2"/>
     </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:46" x14ac:dyDescent="0.3">
       <c r="C4" s="14"/>
       <c r="K4" s="14"/>
       <c r="V4" s="14"/>
       <c r="AD4" s="6"/>
       <c r="AG4" s="14"/>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.3">
       <c r="C5" s="14"/>
       <c r="F5" s="4"/>
       <c r="K5" s="14"/>
@@ -1447,26 +1449,26 @@
       <c r="AG5" s="14"/>
       <c r="AS5" s="2"/>
     </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.3">
       <c r="C6" s="14"/>
       <c r="K6" s="14"/>
       <c r="V6" s="14"/>
       <c r="AG6" s="14"/>
     </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:46" x14ac:dyDescent="0.3">
       <c r="C7" s="14"/>
       <c r="K7" s="14"/>
       <c r="V7" s="14"/>
       <c r="AG7" s="14"/>
       <c r="AS7" s="2"/>
     </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:46" x14ac:dyDescent="0.3">
       <c r="C8" s="14"/>
       <c r="K8" s="14"/>
       <c r="V8" s="14"/>
       <c r="AG8" s="14"/>
     </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:46" x14ac:dyDescent="0.3">
       <c r="C9" s="14"/>
       <c r="K9" s="14"/>
       <c r="M9" s="1" t="s">
@@ -1484,7 +1486,7 @@
       </c>
       <c r="AG9" s="14"/>
     </row>
-    <row r="10" spans="1:46" ht="15" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:46" ht="16" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>0</v>
       </c>
@@ -1571,7 +1573,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:46" ht="30" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:46" ht="28" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
@@ -1634,7 +1636,7 @@
       </c>
       <c r="AG11" s="14"/>
     </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>2022</v>
       </c>
@@ -1704,7 +1706,7 @@
       <c r="AR12" s="6"/>
       <c r="AS12" s="6"/>
     </row>
-    <row r="13" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <f>+A12+1</f>
         <v>2023</v>
@@ -1750,7 +1752,7 @@
       <c r="AR13" s="6"/>
       <c r="AS13" s="6"/>
     </row>
-    <row r="14" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <f>+A13+1</f>
         <v>2024</v>
@@ -1796,7 +1798,7 @@
       <c r="AR14" s="6"/>
       <c r="AS14" s="6"/>
     </row>
-    <row r="15" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <f t="shared" ref="A15:A78" si="0">+A14+1</f>
         <v>2025</v>
@@ -1842,7 +1844,7 @@
       <c r="AR15" s="6"/>
       <c r="AS15" s="6"/>
     </row>
-    <row r="16" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <f t="shared" si="0"/>
         <v>2026</v>
@@ -1888,7 +1890,7 @@
       <c r="AR16" s="6"/>
       <c r="AS16" s="6"/>
     </row>
-    <row r="17" spans="1:45" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <f t="shared" si="0"/>
         <v>2027</v>
@@ -1934,7 +1936,7 @@
       <c r="AR17" s="6"/>
       <c r="AS17" s="6"/>
     </row>
-    <row r="18" spans="1:45" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <f t="shared" si="0"/>
         <v>2028</v>
@@ -1980,7 +1982,7 @@
       <c r="AR18" s="6"/>
       <c r="AS18" s="6"/>
     </row>
-    <row r="19" spans="1:45" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <f t="shared" si="0"/>
         <v>2029</v>
@@ -2026,7 +2028,7 @@
       <c r="AR19" s="6"/>
       <c r="AS19" s="6"/>
     </row>
-    <row r="20" spans="1:45" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <f t="shared" si="0"/>
         <v>2030</v>
@@ -2072,7 +2074,7 @@
       <c r="AR20" s="6"/>
       <c r="AS20" s="6"/>
     </row>
-    <row r="21" spans="1:45" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <f t="shared" si="0"/>
         <v>2031</v>
@@ -2118,7 +2120,7 @@
       <c r="AR21" s="6"/>
       <c r="AS21" s="6"/>
     </row>
-    <row r="22" spans="1:45" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <f t="shared" si="0"/>
         <v>2032</v>
@@ -2164,7 +2166,7 @@
       <c r="AR22" s="6"/>
       <c r="AS22" s="6"/>
     </row>
-    <row r="23" spans="1:45" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <f t="shared" si="0"/>
         <v>2033</v>
@@ -2210,7 +2212,7 @@
       <c r="AR23" s="6"/>
       <c r="AS23" s="6"/>
     </row>
-    <row r="24" spans="1:45" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <f t="shared" si="0"/>
         <v>2034</v>
@@ -2256,7 +2258,7 @@
       <c r="AR24" s="6"/>
       <c r="AS24" s="6"/>
     </row>
-    <row r="25" spans="1:45" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <f t="shared" si="0"/>
         <v>2035</v>
@@ -2302,7 +2304,7 @@
       <c r="AR25" s="6"/>
       <c r="AS25" s="6"/>
     </row>
-    <row r="26" spans="1:45" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <f t="shared" si="0"/>
         <v>2036</v>
@@ -2348,7 +2350,7 @@
       <c r="AR26" s="6"/>
       <c r="AS26" s="6"/>
     </row>
-    <row r="27" spans="1:45" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <f t="shared" si="0"/>
         <v>2037</v>
@@ -2394,7 +2396,7 @@
       <c r="AR27" s="6"/>
       <c r="AS27" s="6"/>
     </row>
-    <row r="28" spans="1:45" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <f t="shared" si="0"/>
         <v>2038</v>
@@ -2440,7 +2442,7 @@
       <c r="AR28" s="6"/>
       <c r="AS28" s="6"/>
     </row>
-    <row r="29" spans="1:45" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <f t="shared" si="0"/>
         <v>2039</v>
@@ -2486,7 +2488,7 @@
       <c r="AR29" s="6"/>
       <c r="AS29" s="6"/>
     </row>
-    <row r="30" spans="1:45" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <f t="shared" si="0"/>
         <v>2040</v>
@@ -2532,7 +2534,7 @@
       <c r="AR30" s="6"/>
       <c r="AS30" s="6"/>
     </row>
-    <row r="31" spans="1:45" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <f t="shared" si="0"/>
         <v>2041</v>
@@ -2578,7 +2580,7 @@
       <c r="AR31" s="6"/>
       <c r="AS31" s="6"/>
     </row>
-    <row r="32" spans="1:45" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <f t="shared" si="0"/>
         <v>2042</v>
@@ -2624,7 +2626,7 @@
       <c r="AR32" s="6"/>
       <c r="AS32" s="6"/>
     </row>
-    <row r="33" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <f t="shared" si="0"/>
         <v>2043</v>
@@ -2670,7 +2672,7 @@
       <c r="AR33" s="6"/>
       <c r="AS33" s="6"/>
     </row>
-    <row r="34" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <f t="shared" si="0"/>
         <v>2044</v>
@@ -2716,7 +2718,7 @@
       <c r="AR34" s="6"/>
       <c r="AS34" s="6"/>
     </row>
-    <row r="35" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <f t="shared" si="0"/>
         <v>2045</v>
@@ -2762,7 +2764,7 @@
       <c r="AR35" s="6"/>
       <c r="AS35" s="6"/>
     </row>
-    <row r="36" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <f t="shared" si="0"/>
         <v>2046</v>
@@ -2808,7 +2810,7 @@
       <c r="AR36" s="6"/>
       <c r="AS36" s="6"/>
     </row>
-    <row r="37" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <f t="shared" si="0"/>
         <v>2047</v>
@@ -2854,7 +2856,7 @@
       <c r="AR37" s="6"/>
       <c r="AS37" s="6"/>
     </row>
-    <row r="38" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <f t="shared" si="0"/>
         <v>2048</v>
@@ -2900,7 +2902,7 @@
       <c r="AR38" s="6"/>
       <c r="AS38" s="6"/>
     </row>
-    <row r="39" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <f t="shared" si="0"/>
         <v>2049</v>
@@ -2946,7 +2948,7 @@
       <c r="AR39" s="6"/>
       <c r="AS39" s="6"/>
     </row>
-    <row r="40" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <f t="shared" si="0"/>
         <v>2050</v>
@@ -2992,7 +2994,7 @@
       <c r="AR40" s="6"/>
       <c r="AS40" s="6"/>
     </row>
-    <row r="41" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <f t="shared" si="0"/>
         <v>2051</v>
@@ -3038,7 +3040,7 @@
       <c r="AR41" s="6"/>
       <c r="AS41" s="6"/>
     </row>
-    <row r="42" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <f t="shared" si="0"/>
         <v>2052</v>
@@ -3084,7 +3086,7 @@
       <c r="AR42" s="6"/>
       <c r="AS42" s="6"/>
     </row>
-    <row r="43" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <f t="shared" si="0"/>
         <v>2053</v>
@@ -3133,7 +3135,7 @@
       <c r="AU43" s="6"/>
       <c r="AV43" s="6"/>
     </row>
-    <row r="44" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <f t="shared" si="0"/>
         <v>2054</v>
@@ -3182,7 +3184,7 @@
       <c r="AU44" s="6"/>
       <c r="AV44" s="6"/>
     </row>
-    <row r="45" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <f t="shared" si="0"/>
         <v>2055</v>
@@ -3231,7 +3233,7 @@
       <c r="AU45" s="6"/>
       <c r="AV45" s="6"/>
     </row>
-    <row r="46" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <f t="shared" si="0"/>
         <v>2056</v>
@@ -3280,7 +3282,7 @@
       <c r="AU46" s="6"/>
       <c r="AV46" s="6"/>
     </row>
-    <row r="47" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <f t="shared" si="0"/>
         <v>2057</v>
@@ -3329,7 +3331,7 @@
       <c r="AU47" s="6"/>
       <c r="AV47" s="6"/>
     </row>
-    <row r="48" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <f t="shared" si="0"/>
         <v>2058</v>
@@ -3378,7 +3380,7 @@
       <c r="AU48" s="6"/>
       <c r="AV48" s="6"/>
     </row>
-    <row r="49" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <f t="shared" si="0"/>
         <v>2059</v>
@@ -3427,7 +3429,7 @@
       <c r="AU49" s="6"/>
       <c r="AV49" s="6"/>
     </row>
-    <row r="50" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <f t="shared" si="0"/>
         <v>2060</v>
@@ -3476,7 +3478,7 @@
       <c r="AU50" s="6"/>
       <c r="AV50" s="6"/>
     </row>
-    <row r="51" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <f t="shared" si="0"/>
         <v>2061</v>
@@ -3525,7 +3527,7 @@
       <c r="AU51" s="6"/>
       <c r="AV51" s="6"/>
     </row>
-    <row r="52" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <f t="shared" si="0"/>
         <v>2062</v>
@@ -3574,7 +3576,7 @@
       <c r="AU52" s="6"/>
       <c r="AV52" s="6"/>
     </row>
-    <row r="53" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <f t="shared" si="0"/>
         <v>2063</v>
@@ -3623,7 +3625,7 @@
       <c r="AU53" s="6"/>
       <c r="AV53" s="6"/>
     </row>
-    <row r="54" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <f t="shared" si="0"/>
         <v>2064</v>
@@ -3669,7 +3671,7 @@
       <c r="AR54" s="6"/>
       <c r="AS54" s="6"/>
     </row>
-    <row r="55" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <f t="shared" si="0"/>
         <v>2065</v>
@@ -3715,7 +3717,7 @@
       <c r="AR55" s="6"/>
       <c r="AS55" s="6"/>
     </row>
-    <row r="56" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <f t="shared" si="0"/>
         <v>2066</v>
@@ -3761,7 +3763,7 @@
       <c r="AR56" s="6"/>
       <c r="AS56" s="6"/>
     </row>
-    <row r="57" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <f t="shared" si="0"/>
         <v>2067</v>
@@ -3807,7 +3809,7 @@
       <c r="AR57" s="6"/>
       <c r="AS57" s="6"/>
     </row>
-    <row r="58" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <f t="shared" si="0"/>
         <v>2068</v>
@@ -3853,7 +3855,7 @@
       <c r="AR58" s="6"/>
       <c r="AS58" s="6"/>
     </row>
-    <row r="59" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <f t="shared" si="0"/>
         <v>2069</v>
@@ -3899,7 +3901,7 @@
       <c r="AR59" s="6"/>
       <c r="AS59" s="6"/>
     </row>
-    <row r="60" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <f t="shared" si="0"/>
         <v>2070</v>
@@ -3945,7 +3947,7 @@
       <c r="AR60" s="6"/>
       <c r="AS60" s="6"/>
     </row>
-    <row r="61" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <f t="shared" si="0"/>
         <v>2071</v>
@@ -3991,7 +3993,7 @@
       <c r="AR61" s="6"/>
       <c r="AS61" s="6"/>
     </row>
-    <row r="62" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <f t="shared" si="0"/>
         <v>2072</v>
@@ -4037,7 +4039,7 @@
       <c r="AR62" s="6"/>
       <c r="AS62" s="6"/>
     </row>
-    <row r="63" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <f t="shared" si="0"/>
         <v>2073</v>
@@ -4083,7 +4085,7 @@
       <c r="AR63" s="6"/>
       <c r="AS63" s="6"/>
     </row>
-    <row r="64" spans="1:48" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <f t="shared" si="0"/>
         <v>2074</v>
@@ -4129,7 +4131,7 @@
       <c r="AR64" s="6"/>
       <c r="AS64" s="6"/>
     </row>
-    <row r="65" spans="1:45" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <f t="shared" si="0"/>
         <v>2075</v>
@@ -4175,7 +4177,7 @@
       <c r="AR65" s="6"/>
       <c r="AS65" s="6"/>
     </row>
-    <row r="66" spans="1:45" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <f t="shared" si="0"/>
         <v>2076</v>
@@ -4221,7 +4223,7 @@
       <c r="AR66" s="6"/>
       <c r="AS66" s="6"/>
     </row>
-    <row r="67" spans="1:45" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <f t="shared" si="0"/>
         <v>2077</v>
@@ -4267,7 +4269,7 @@
       <c r="AR67" s="6"/>
       <c r="AS67" s="6"/>
     </row>
-    <row r="68" spans="1:45" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <f t="shared" si="0"/>
         <v>2078</v>
@@ -4313,7 +4315,7 @@
       <c r="AR68" s="6"/>
       <c r="AS68" s="6"/>
     </row>
-    <row r="69" spans="1:45" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <f t="shared" si="0"/>
         <v>2079</v>
@@ -4359,7 +4361,7 @@
       <c r="AR69" s="6"/>
       <c r="AS69" s="6"/>
     </row>
-    <row r="70" spans="1:45" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <f t="shared" si="0"/>
         <v>2080</v>
@@ -4397,7 +4399,7 @@
       <c r="AK70" s="3"/>
       <c r="AL70" s="3"/>
     </row>
-    <row r="71" spans="1:45" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <f t="shared" si="0"/>
         <v>2081</v>
@@ -4435,7 +4437,7 @@
       <c r="AK71" s="3"/>
       <c r="AL71" s="3"/>
     </row>
-    <row r="72" spans="1:45" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <f t="shared" si="0"/>
         <v>2082</v>
@@ -4473,7 +4475,7 @@
       <c r="AK72" s="3"/>
       <c r="AL72" s="3"/>
     </row>
-    <row r="73" spans="1:45" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <f t="shared" si="0"/>
         <v>2083</v>
@@ -4511,7 +4513,7 @@
       <c r="AK73" s="3"/>
       <c r="AL73" s="3"/>
     </row>
-    <row r="74" spans="1:45" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <f t="shared" si="0"/>
         <v>2084</v>
@@ -4549,7 +4551,7 @@
       <c r="AK74" s="3"/>
       <c r="AL74" s="3"/>
     </row>
-    <row r="75" spans="1:45" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <f t="shared" si="0"/>
         <v>2085</v>
@@ -4587,7 +4589,7 @@
       <c r="AK75" s="3"/>
       <c r="AL75" s="3"/>
     </row>
-    <row r="76" spans="1:45" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <f t="shared" si="0"/>
         <v>2086</v>
@@ -4625,7 +4627,7 @@
       <c r="AK76" s="3"/>
       <c r="AL76" s="3"/>
     </row>
-    <row r="77" spans="1:45" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <f t="shared" si="0"/>
         <v>2087</v>
@@ -4663,7 +4665,7 @@
       <c r="AK77" s="3"/>
       <c r="AL77" s="3"/>
     </row>
-    <row r="78" spans="1:45" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <f t="shared" si="0"/>
         <v>2088</v>
@@ -4701,7 +4703,7 @@
       <c r="AK78" s="3"/>
       <c r="AL78" s="3"/>
     </row>
-    <row r="79" spans="1:45" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <f t="shared" ref="A79:A92" si="1">+A78+1</f>
         <v>2089</v>
@@ -4739,7 +4741,7 @@
       <c r="AK79" s="3"/>
       <c r="AL79" s="3"/>
     </row>
-    <row r="80" spans="1:45" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <f t="shared" si="1"/>
         <v>2090</v>
@@ -4777,7 +4779,7 @@
       <c r="AK80" s="3"/>
       <c r="AL80" s="3"/>
     </row>
-    <row r="81" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <f t="shared" si="1"/>
         <v>2091</v>
@@ -4815,7 +4817,7 @@
       <c r="AK81" s="3"/>
       <c r="AL81" s="3"/>
     </row>
-    <row r="82" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <f t="shared" si="1"/>
         <v>2092</v>
@@ -4853,7 +4855,7 @@
       <c r="AK82" s="3"/>
       <c r="AL82" s="3"/>
     </row>
-    <row r="83" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <f t="shared" si="1"/>
         <v>2093</v>
@@ -4891,7 +4893,7 @@
       <c r="AK83" s="3"/>
       <c r="AL83" s="3"/>
     </row>
-    <row r="84" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <f t="shared" si="1"/>
         <v>2094</v>
@@ -4929,7 +4931,7 @@
       <c r="AK84" s="3"/>
       <c r="AL84" s="3"/>
     </row>
-    <row r="85" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <f t="shared" si="1"/>
         <v>2095</v>
@@ -4967,7 +4969,7 @@
       <c r="AK85" s="3"/>
       <c r="AL85" s="3"/>
     </row>
-    <row r="86" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <f t="shared" si="1"/>
         <v>2096</v>
@@ -5005,7 +5007,7 @@
       <c r="AK86" s="3"/>
       <c r="AL86" s="3"/>
     </row>
-    <row r="87" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <f t="shared" si="1"/>
         <v>2097</v>
@@ -5043,7 +5045,7 @@
       <c r="AK87" s="3"/>
       <c r="AL87" s="3"/>
     </row>
-    <row r="88" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <f t="shared" si="1"/>
         <v>2098</v>
@@ -5081,7 +5083,7 @@
       <c r="AK88" s="3"/>
       <c r="AL88" s="3"/>
     </row>
-    <row r="89" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <f t="shared" si="1"/>
         <v>2099</v>
@@ -5119,7 +5121,7 @@
       <c r="AK89" s="3"/>
       <c r="AL89" s="3"/>
     </row>
-    <row r="90" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <f t="shared" si="1"/>
         <v>2100</v>
@@ -5157,7 +5159,7 @@
       <c r="AK90" s="3"/>
       <c r="AL90" s="3"/>
     </row>
-    <row r="91" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <f t="shared" si="1"/>
         <v>2101</v>
@@ -5195,7 +5197,7 @@
       <c r="AK91" s="3"/>
       <c r="AL91" s="3"/>
     </row>
-    <row r="92" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <f t="shared" si="1"/>
         <v>2102</v>
@@ -5233,7 +5235,7 @@
       <c r="AK92" s="3"/>
       <c r="AL92" s="3"/>
     </row>
-    <row r="93" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:38" x14ac:dyDescent="0.3">
       <c r="B93" s="5"/>
       <c r="E93" s="3"/>
       <c r="F93" s="3"/>
@@ -5249,7 +5251,7 @@
       <c r="T93" s="3"/>
       <c r="U93" s="3"/>
     </row>
-    <row r="94" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:38" x14ac:dyDescent="0.3">
       <c r="B94" s="5"/>
       <c r="E94" s="3"/>
       <c r="F94" s="3"/>
@@ -5265,7 +5267,7 @@
       <c r="T94" s="3"/>
       <c r="U94" s="3"/>
     </row>
-    <row r="95" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:38" x14ac:dyDescent="0.3">
       <c r="B95" s="5"/>
       <c r="E95" s="3"/>
       <c r="F95" s="3"/>
@@ -5281,7 +5283,7 @@
       <c r="T95" s="3"/>
       <c r="U95" s="3"/>
     </row>
-    <row r="96" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:38" x14ac:dyDescent="0.3">
       <c r="B96" s="5"/>
       <c r="E96" s="3"/>
       <c r="F96" s="3"/>
@@ -5297,7 +5299,7 @@
       <c r="T96" s="3"/>
       <c r="U96" s="3"/>
     </row>
-    <row r="97" spans="2:21" x14ac:dyDescent="0.15">
+    <row r="97" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B97" s="5"/>
       <c r="E97" s="3"/>
       <c r="F97" s="3"/>
@@ -5313,7 +5315,7 @@
       <c r="T97" s="3"/>
       <c r="U97" s="3"/>
     </row>
-    <row r="98" spans="2:21" x14ac:dyDescent="0.15">
+    <row r="98" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B98" s="5"/>
       <c r="E98" s="3"/>
       <c r="F98" s="3"/>
@@ -5329,7 +5331,7 @@
       <c r="T98" s="3"/>
       <c r="U98" s="3"/>
     </row>
-    <row r="99" spans="2:21" x14ac:dyDescent="0.15">
+    <row r="99" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B99" s="5"/>
       <c r="E99" s="3"/>
       <c r="F99" s="3"/>
@@ -5345,7 +5347,7 @@
       <c r="T99" s="3"/>
       <c r="U99" s="3"/>
     </row>
-    <row r="100" spans="2:21" x14ac:dyDescent="0.15">
+    <row r="100" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B100" s="5"/>
       <c r="E100" s="3"/>
       <c r="F100" s="3"/>
@@ -5361,7 +5363,7 @@
       <c r="T100" s="3"/>
       <c r="U100" s="3"/>
     </row>
-    <row r="101" spans="2:21" x14ac:dyDescent="0.15">
+    <row r="101" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B101" s="5"/>
       <c r="E101" s="3"/>
       <c r="F101" s="3"/>
@@ -5377,7 +5379,7 @@
       <c r="T101" s="3"/>
       <c r="U101" s="3"/>
     </row>
-    <row r="102" spans="2:21" x14ac:dyDescent="0.15">
+    <row r="102" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B102" s="5"/>
       <c r="E102" s="3"/>
       <c r="F102" s="3"/>
@@ -5393,7 +5395,7 @@
       <c r="T102" s="3"/>
       <c r="U102" s="3"/>
     </row>
-    <row r="103" spans="2:21" x14ac:dyDescent="0.15">
+    <row r="103" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B103" s="5"/>
       <c r="E103" s="3"/>
       <c r="F103" s="3"/>
@@ -5409,7 +5411,7 @@
       <c r="T103" s="3"/>
       <c r="U103" s="3"/>
     </row>
-    <row r="104" spans="2:21" x14ac:dyDescent="0.15">
+    <row r="104" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B104" s="5"/>
       <c r="E104" s="3"/>
       <c r="F104" s="3"/>
@@ -5425,7 +5427,7 @@
       <c r="T104" s="3"/>
       <c r="U104" s="3"/>
     </row>
-    <row r="105" spans="2:21" x14ac:dyDescent="0.15">
+    <row r="105" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B105" s="5"/>
       <c r="E105" s="3"/>
       <c r="F105" s="3"/>
@@ -5441,7 +5443,7 @@
       <c r="T105" s="3"/>
       <c r="U105" s="3"/>
     </row>
-    <row r="106" spans="2:21" x14ac:dyDescent="0.15">
+    <row r="106" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B106" s="5"/>
       <c r="E106" s="3"/>
       <c r="F106" s="3"/>
@@ -5457,7 +5459,7 @@
       <c r="T106" s="3"/>
       <c r="U106" s="3"/>
     </row>
-    <row r="107" spans="2:21" x14ac:dyDescent="0.15">
+    <row r="107" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B107" s="5"/>
       <c r="E107" s="3"/>
       <c r="F107" s="3"/>
@@ -5473,7 +5475,7 @@
       <c r="T107" s="3"/>
       <c r="U107" s="3"/>
     </row>
-    <row r="108" spans="2:21" x14ac:dyDescent="0.15">
+    <row r="108" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B108" s="5"/>
       <c r="E108" s="3"/>
       <c r="F108" s="3"/>
@@ -5489,7 +5491,7 @@
       <c r="T108" s="3"/>
       <c r="U108" s="3"/>
     </row>
-    <row r="109" spans="2:21" x14ac:dyDescent="0.15">
+    <row r="109" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B109" s="5"/>
       <c r="E109" s="3"/>
       <c r="F109" s="3"/>
@@ -5505,7 +5507,7 @@
       <c r="T109" s="3"/>
       <c r="U109" s="3"/>
     </row>
-    <row r="110" spans="2:21" x14ac:dyDescent="0.15">
+    <row r="110" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B110" s="5"/>
       <c r="E110" s="3"/>
       <c r="F110" s="3"/>
@@ -5521,7 +5523,7 @@
       <c r="T110" s="3"/>
       <c r="U110" s="3"/>
     </row>
-    <row r="111" spans="2:21" x14ac:dyDescent="0.15">
+    <row r="111" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B111" s="5"/>
       <c r="E111" s="3"/>
       <c r="F111" s="3"/>
@@ -5537,7 +5539,7 @@
       <c r="T111" s="3"/>
       <c r="U111" s="3"/>
     </row>
-    <row r="112" spans="2:21" x14ac:dyDescent="0.15">
+    <row r="112" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B112" s="5"/>
       <c r="E112" s="3"/>
       <c r="F112" s="3"/>
@@ -5553,7 +5555,7 @@
       <c r="T112" s="3"/>
       <c r="U112" s="3"/>
     </row>
-    <row r="113" spans="2:21" x14ac:dyDescent="0.15">
+    <row r="113" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B113" s="5"/>
       <c r="E113" s="3"/>
       <c r="F113" s="3"/>
@@ -5569,7 +5571,7 @@
       <c r="T113" s="3"/>
       <c r="U113" s="3"/>
     </row>
-    <row r="114" spans="2:21" x14ac:dyDescent="0.15">
+    <row r="114" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B114" s="5"/>
       <c r="E114" s="3"/>
       <c r="F114" s="3"/>
@@ -5585,7 +5587,7 @@
       <c r="T114" s="3"/>
       <c r="U114" s="3"/>
     </row>
-    <row r="115" spans="2:21" x14ac:dyDescent="0.15">
+    <row r="115" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B115" s="5"/>
       <c r="E115" s="3"/>
       <c r="F115" s="3"/>
@@ -5601,7 +5603,7 @@
       <c r="T115" s="3"/>
       <c r="U115" s="3"/>
     </row>
-    <row r="116" spans="2:21" x14ac:dyDescent="0.15">
+    <row r="116" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B116" s="5"/>
       <c r="E116" s="3"/>
       <c r="F116" s="3"/>
@@ -5617,7 +5619,7 @@
       <c r="T116" s="3"/>
       <c r="U116" s="3"/>
     </row>
-    <row r="117" spans="2:21" x14ac:dyDescent="0.15">
+    <row r="117" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B117" s="5"/>
       <c r="E117" s="3"/>
       <c r="F117" s="3"/>
@@ -5633,7 +5635,7 @@
       <c r="T117" s="3"/>
       <c r="U117" s="3"/>
     </row>
-    <row r="118" spans="2:21" x14ac:dyDescent="0.15">
+    <row r="118" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B118" s="5"/>
       <c r="E118" s="3"/>
       <c r="F118" s="3"/>
@@ -5649,7 +5651,7 @@
       <c r="T118" s="3"/>
       <c r="U118" s="3"/>
     </row>
-    <row r="119" spans="2:21" x14ac:dyDescent="0.15">
+    <row r="119" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B119" s="5"/>
       <c r="E119" s="3"/>
       <c r="F119" s="3"/>
@@ -5665,7 +5667,7 @@
       <c r="T119" s="3"/>
       <c r="U119" s="3"/>
     </row>
-    <row r="120" spans="2:21" x14ac:dyDescent="0.15">
+    <row r="120" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B120" s="5"/>
       <c r="E120" s="3"/>
       <c r="F120" s="3"/>
@@ -5692,21 +5694,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B407838-5EEB-6943-BFD7-2887BDD23C1A}">
   <dimension ref="A1:K96"/>
   <sheetViews>
-    <sheetView zoomScale="144" workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="16384" width="10.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" s="20" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>28</v>
       </c>
@@ -5738,7 +5740,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B10" s="7" t="s">
         <v>10</v>
       </c>
@@ -5770,7 +5772,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>26</v>
       </c>
@@ -5802,7 +5804,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>2022</v>
       </c>
@@ -5837,7 +5839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <f>+A12+1</f>
         <v>2023</v>
@@ -5873,7 +5875,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <f>+A13+1</f>
         <v>2024</v>
@@ -5909,7 +5911,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <f t="shared" ref="A15:A78" si="0">+A14+1</f>
         <v>2025</v>
@@ -5945,7 +5947,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <f t="shared" si="0"/>
         <v>2026</v>
@@ -5981,7 +5983,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <f t="shared" si="0"/>
         <v>2027</v>
@@ -6017,7 +6019,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <f t="shared" si="0"/>
         <v>2028</v>
@@ -6053,7 +6055,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <f t="shared" si="0"/>
         <v>2029</v>
@@ -6089,7 +6091,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <f t="shared" si="0"/>
         <v>2030</v>
@@ -6125,7 +6127,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <f t="shared" si="0"/>
         <v>2031</v>
@@ -6161,7 +6163,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <f t="shared" si="0"/>
         <v>2032</v>
@@ -6197,7 +6199,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <f t="shared" si="0"/>
         <v>2033</v>
@@ -6233,7 +6235,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <f t="shared" si="0"/>
         <v>2034</v>
@@ -6269,7 +6271,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <f t="shared" si="0"/>
         <v>2035</v>
@@ -6305,7 +6307,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <f t="shared" si="0"/>
         <v>2036</v>
@@ -6341,7 +6343,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <f t="shared" si="0"/>
         <v>2037</v>
@@ -6377,7 +6379,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <f t="shared" si="0"/>
         <v>2038</v>
@@ -6413,7 +6415,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <f t="shared" si="0"/>
         <v>2039</v>
@@ -6449,7 +6451,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <f t="shared" si="0"/>
         <v>2040</v>
@@ -6485,7 +6487,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <f t="shared" si="0"/>
         <v>2041</v>
@@ -6521,7 +6523,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <f t="shared" si="0"/>
         <v>2042</v>
@@ -6557,7 +6559,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <f t="shared" si="0"/>
         <v>2043</v>
@@ -6593,7 +6595,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <f t="shared" si="0"/>
         <v>2044</v>
@@ -6629,7 +6631,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <f t="shared" si="0"/>
         <v>2045</v>
@@ -6665,7 +6667,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <f t="shared" si="0"/>
         <v>2046</v>
@@ -6701,7 +6703,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <f t="shared" si="0"/>
         <v>2047</v>
@@ -6737,7 +6739,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <f t="shared" si="0"/>
         <v>2048</v>
@@ -6773,7 +6775,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <f t="shared" si="0"/>
         <v>2049</v>
@@ -6809,7 +6811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <f t="shared" si="0"/>
         <v>2050</v>
@@ -6845,7 +6847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <f t="shared" si="0"/>
         <v>2051</v>
@@ -6881,7 +6883,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <f t="shared" si="0"/>
         <v>2052</v>
@@ -6917,7 +6919,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <f t="shared" si="0"/>
         <v>2053</v>
@@ -6953,7 +6955,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <f t="shared" si="0"/>
         <v>2054</v>
@@ -6989,7 +6991,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <f t="shared" si="0"/>
         <v>2055</v>
@@ -7025,7 +7027,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <f t="shared" si="0"/>
         <v>2056</v>
@@ -7061,7 +7063,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <f t="shared" si="0"/>
         <v>2057</v>
@@ -7097,7 +7099,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <f t="shared" si="0"/>
         <v>2058</v>
@@ -7133,7 +7135,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <f t="shared" si="0"/>
         <v>2059</v>
@@ -7169,7 +7171,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <f t="shared" si="0"/>
         <v>2060</v>
@@ -7205,7 +7207,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <f t="shared" si="0"/>
         <v>2061</v>
@@ -7241,7 +7243,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <f t="shared" si="0"/>
         <v>2062</v>
@@ -7277,7 +7279,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <f t="shared" si="0"/>
         <v>2063</v>
@@ -7313,7 +7315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <f t="shared" si="0"/>
         <v>2064</v>
@@ -7349,7 +7351,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <f t="shared" si="0"/>
         <v>2065</v>
@@ -7385,7 +7387,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <f t="shared" si="0"/>
         <v>2066</v>
@@ -7421,7 +7423,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <f t="shared" si="0"/>
         <v>2067</v>
@@ -7457,7 +7459,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <f t="shared" si="0"/>
         <v>2068</v>
@@ -7493,7 +7495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <f t="shared" si="0"/>
         <v>2069</v>
@@ -7529,7 +7531,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <f t="shared" si="0"/>
         <v>2070</v>
@@ -7565,7 +7567,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <f t="shared" si="0"/>
         <v>2071</v>
@@ -7601,7 +7603,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <f t="shared" si="0"/>
         <v>2072</v>
@@ -7637,7 +7639,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <f t="shared" si="0"/>
         <v>2073</v>
@@ -7673,7 +7675,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <f t="shared" si="0"/>
         <v>2074</v>
@@ -7709,7 +7711,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <f t="shared" si="0"/>
         <v>2075</v>
@@ -7745,7 +7747,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <f t="shared" si="0"/>
         <v>2076</v>
@@ -7781,7 +7783,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <f t="shared" si="0"/>
         <v>2077</v>
@@ -7817,7 +7819,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <f t="shared" si="0"/>
         <v>2078</v>
@@ -7853,7 +7855,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <f t="shared" si="0"/>
         <v>2079</v>
@@ -7889,7 +7891,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <f t="shared" si="0"/>
         <v>2080</v>
@@ -7925,7 +7927,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <f t="shared" si="0"/>
         <v>2081</v>
@@ -7961,7 +7963,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <f t="shared" si="0"/>
         <v>2082</v>
@@ -7997,7 +7999,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <f t="shared" si="0"/>
         <v>2083</v>
@@ -8033,7 +8035,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <f t="shared" si="0"/>
         <v>2084</v>
@@ -8069,7 +8071,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <f t="shared" si="0"/>
         <v>2085</v>
@@ -8105,7 +8107,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <f t="shared" si="0"/>
         <v>2086</v>
@@ -8141,7 +8143,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <f t="shared" si="0"/>
         <v>2087</v>
@@ -8177,7 +8179,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <f t="shared" si="0"/>
         <v>2088</v>
@@ -8213,7 +8215,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <f t="shared" ref="A79:A92" si="1">+A78+1</f>
         <v>2089</v>
@@ -8249,7 +8251,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <f t="shared" si="1"/>
         <v>2090</v>
@@ -8285,7 +8287,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <f t="shared" si="1"/>
         <v>2091</v>
@@ -8321,7 +8323,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <f t="shared" si="1"/>
         <v>2092</v>
@@ -8357,7 +8359,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <f t="shared" si="1"/>
         <v>2093</v>
@@ -8393,7 +8395,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <f t="shared" si="1"/>
         <v>2094</v>
@@ -8429,7 +8431,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <f t="shared" si="1"/>
         <v>2095</v>
@@ -8465,7 +8467,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <f t="shared" si="1"/>
         <v>2096</v>
@@ -8501,7 +8503,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <f t="shared" si="1"/>
         <v>2097</v>
@@ -8537,7 +8539,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <f t="shared" si="1"/>
         <v>2098</v>
@@ -8573,7 +8575,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <f t="shared" si="1"/>
         <v>2099</v>
@@ -8609,7 +8611,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <f t="shared" si="1"/>
         <v>2100</v>
@@ -8645,7 +8647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <f t="shared" si="1"/>
         <v>2101</v>
@@ -8681,7 +8683,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <f t="shared" si="1"/>
         <v>2102</v>
@@ -8717,7 +8719,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B94" s="6"/>
       <c r="C94" s="6"/>
       <c r="D94" s="6"/>
@@ -8729,7 +8731,7 @@
       <c r="J94" s="6"/>
       <c r="K94" s="6"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B95" s="6"/>
       <c r="C95" s="6"/>
       <c r="D95" s="6"/>
@@ -8741,7 +8743,7 @@
       <c r="J95" s="6"/>
       <c r="K95" s="6"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B96" s="6"/>
       <c r="C96" s="6"/>
       <c r="D96" s="6"/>

</xml_diff>